<commit_message>
act 08-08-2025 se agregan mas equipos y nueva funcionalidad
</commit_message>
<xml_diff>
--- a/new-stats/adc-juan-pablo-ii-college.xlsx
+++ b/new-stats/adc-juan-pablo-ii-college.xlsx
@@ -1730,22 +1730,62 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>05/08/2025</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Melgar</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Juan Pablo II</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="M23" t="n">
+        <v>5</v>
+      </c>
+      <c r="N23" t="n">
+        <v>21</v>
+      </c>
+      <c r="O23" t="n">
+        <v>2</v>
+      </c>
+      <c r="P23" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>

</xml_diff>